<commit_message>
added background soil percentiles
</commit_message>
<xml_diff>
--- a/R/vanta_xrf_elements.xlsx
+++ b/R/vanta_xrf_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usdagcc-my.sharepoint.com/personal/samuel_araya_usda_gov/Documents/Documents/R-Project/TidyXRF/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_907D5B90573D742009BE52CE1DD4F65D38A92CDB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B1D430C-90DE-41E1-87E2-3CE35F337F9A}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="11_907D5B90573D742009BE52CE1DD4F65D38A92CDB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86F776A1-3E5E-4493-BC8C-52E79E61D0BE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="xrf_elements" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="170">
   <si>
     <t>Atomic_Number</t>
   </si>
@@ -511,9 +511,6 @@
     <t>EPA (2003) Guidance for Developing Ecological Soil Screening Levels (Eco-SSLs), URL: https://www.epa.gov/chemical-research/guidance-developing-ecological-soil-screening-levels, Accessed: 05/20/2022</t>
   </si>
   <si>
-    <t>US Soil Background</t>
-  </si>
-  <si>
     <t>NJ DEP Soil Remediation</t>
   </si>
   <si>
@@ -526,7 +523,28 @@
     <t>Residential guidelines of NYS Dept. of Envt. Conservation, and  Dept. of Health. (http://cwmi.css.cornell.edu/Metals_Urban_Garden_Soils.pdf)</t>
   </si>
   <si>
-    <t>US Median Background Soil Concentration for Metals. (EPA 2003, Eco-SSLs)</t>
+    <t>US Soil Median</t>
+  </si>
+  <si>
+    <t>US Soil 75th Percentile</t>
+  </si>
+  <si>
+    <t>US Soil 90th Percentile</t>
+  </si>
+  <si>
+    <t>US Soil 99th Percentile</t>
+  </si>
+  <si>
+    <t>50th percentile value of US background soil concentration for metals. (EPA 2003, Eco-SSLs)</t>
+  </si>
+  <si>
+    <t>75th percentile value of US background soil concentration for metals. (EPA 2003, Eco-SSLs)</t>
+  </si>
+  <si>
+    <t>90th percentile value of US background soil concentration for metals. (EPA 2003, Eco-SSLs)</t>
+  </si>
+  <si>
+    <t>99th percentile value of US background soil concentration for metals. (EPA 2003, Eco-SSLs)</t>
   </si>
 </sst>
 </file>
@@ -969,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -986,10 +1004,10 @@
     <col min="7" max="7" width="8.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5703125" style="1"/>
+    <col min="13" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1009,16 +1027,25 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+      <c r="J1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K1" t="s">
+        <v>164</v>
+      </c>
+      <c r="L1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>12</v>
       </c>
@@ -1037,8 +1064,17 @@
       <c r="I2">
         <v>5500</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>10000</v>
+      </c>
+      <c r="K2">
+        <v>11200</v>
+      </c>
+      <c r="L2">
+        <v>14040</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>13</v>
       </c>
@@ -1057,8 +1093,17 @@
       <c r="I3">
         <v>49000</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>64000</v>
+      </c>
+      <c r="K3">
+        <v>72700</v>
+      </c>
+      <c r="L3">
+        <v>95850</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>14</v>
       </c>
@@ -1077,8 +1122,17 @@
       <c r="I4">
         <v>310000</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>360000</v>
+      </c>
+      <c r="K4">
+        <v>370000</v>
+      </c>
+      <c r="L4">
+        <v>390000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>15</v>
       </c>
@@ -1099,8 +1153,17 @@
       <c r="I5">
         <v>340</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>530</v>
+      </c>
+      <c r="K5">
+        <v>724</v>
+      </c>
+      <c r="L5">
+        <v>852.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>16</v>
       </c>
@@ -1121,8 +1184,17 @@
       <c r="I6">
         <v>820</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>870</v>
+      </c>
+      <c r="K6">
+        <v>976</v>
+      </c>
+      <c r="L6">
+        <v>2418</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>17</v>
       </c>
@@ -1141,7 +1213,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>19</v>
       </c>
@@ -1162,8 +1234,17 @@
       <c r="I8">
         <v>15000</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>18000</v>
+      </c>
+      <c r="K8">
+        <v>19200</v>
+      </c>
+      <c r="L8">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>20</v>
       </c>
@@ -1184,8 +1265,17 @@
       <c r="I9">
         <v>9200</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>24000</v>
+      </c>
+      <c r="K9">
+        <v>29600</v>
+      </c>
+      <c r="L9">
+        <v>53440</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>21</v>
       </c>
@@ -1204,8 +1294,17 @@
       <c r="I10">
         <v>8.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <v>12</v>
+      </c>
+      <c r="L10">
+        <v>16.559999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>22</v>
       </c>
@@ -1224,8 +1323,17 @@
       <c r="I11">
         <v>2900</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>3500</v>
+      </c>
+      <c r="K11">
+        <v>4640</v>
+      </c>
+      <c r="L11">
+        <v>6016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>23</v>
       </c>
@@ -1244,8 +1352,17 @@
       <c r="I12">
         <v>69</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>83.25</v>
+      </c>
+      <c r="K12">
+        <v>110</v>
+      </c>
+      <c r="L12">
+        <v>184.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>24</v>
       </c>
@@ -1271,8 +1388,17 @@
       <c r="I13">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>55</v>
+      </c>
+      <c r="K13">
+        <v>67</v>
+      </c>
+      <c r="L13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>25</v>
       </c>
@@ -1297,8 +1423,17 @@
       <c r="I14">
         <v>470</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>610</v>
+      </c>
+      <c r="K14">
+        <v>840</v>
+      </c>
+      <c r="L14">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>26</v>
       </c>
@@ -1319,8 +1454,17 @@
       <c r="I15">
         <v>23000</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>29000</v>
+      </c>
+      <c r="K15">
+        <v>37000</v>
+      </c>
+      <c r="L15">
+        <v>51330</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>27</v>
       </c>
@@ -1343,8 +1487,17 @@
       <c r="I16">
         <v>8.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>12</v>
+      </c>
+      <c r="K16">
+        <v>14.4</v>
+      </c>
+      <c r="L16">
+        <v>17.16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>28</v>
       </c>
@@ -1372,8 +1525,17 @@
       <c r="I17">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>23</v>
+      </c>
+      <c r="K17">
+        <v>28</v>
+      </c>
+      <c r="L17">
+        <v>41.96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>29</v>
       </c>
@@ -1401,8 +1563,17 @@
       <c r="I18">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>27</v>
+      </c>
+      <c r="K18">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="L18">
+        <v>49.97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>30</v>
       </c>
@@ -1430,8 +1601,17 @@
       <c r="I19">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>67</v>
+      </c>
+      <c r="K19">
+        <v>79.2</v>
+      </c>
+      <c r="L19">
+        <v>151.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>31</v>
       </c>
@@ -1450,8 +1630,17 @@
       <c r="I20">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>20</v>
+      </c>
+      <c r="K20">
+        <v>24.2</v>
+      </c>
+      <c r="L20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>32</v>
       </c>
@@ -1470,8 +1659,17 @@
       <c r="I21">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>1.4</v>
+      </c>
+      <c r="K21">
+        <v>1.6</v>
+      </c>
+      <c r="L21">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>33</v>
       </c>
@@ -1499,8 +1697,17 @@
       <c r="I22">
         <v>6.65</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>8.5749999999999993</v>
+      </c>
+      <c r="K22">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="L22">
+        <v>14.32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>34</v>
       </c>
@@ -1528,8 +1735,17 @@
       <c r="I23">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>0.5</v>
+      </c>
+      <c r="K23">
+        <v>0.73</v>
+      </c>
+      <c r="L23">
+        <v>2.0209999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>35</v>
       </c>
@@ -1548,8 +1764,17 @@
       <c r="I24">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K24">
+        <v>1.5</v>
+      </c>
+      <c r="L24">
+        <v>5.2160000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>37</v>
       </c>
@@ -1570,8 +1795,17 @@
       <c r="I25">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>82</v>
+      </c>
+      <c r="K25">
+        <v>93.2</v>
+      </c>
+      <c r="L25">
+        <v>115.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>38</v>
       </c>
@@ -1592,8 +1826,17 @@
       <c r="I26">
         <v>130</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>200</v>
+      </c>
+      <c r="K26">
+        <v>293</v>
+      </c>
+      <c r="L26">
+        <v>491.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>39</v>
       </c>
@@ -1612,8 +1855,17 @@
       <c r="I27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>30</v>
+      </c>
+      <c r="K27">
+        <v>33</v>
+      </c>
+      <c r="L27">
+        <v>38.56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>40</v>
       </c>
@@ -1634,8 +1886,17 @@
       <c r="I28">
         <v>220</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>290</v>
+      </c>
+      <c r="K28">
+        <v>322</v>
+      </c>
+      <c r="L28">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>41</v>
       </c>
@@ -1654,8 +1915,17 @@
       <c r="I29">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <v>13</v>
+      </c>
+      <c r="K29">
+        <v>15</v>
+      </c>
+      <c r="L29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>42</v>
       </c>
@@ -1679,8 +1949,17 @@
       <c r="I30">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <v>1.9</v>
+      </c>
+      <c r="K30">
+        <v>2.48</v>
+      </c>
+      <c r="L30">
+        <v>4.1959999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43</v>
       </c>
@@ -1697,7 +1976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>44</v>
       </c>
@@ -1714,7 +1993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>45</v>
       </c>
@@ -1731,7 +2010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>46</v>
       </c>
@@ -1748,7 +2027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>47</v>
       </c>
@@ -1773,8 +2052,17 @@
       <c r="I35">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1.2</v>
+      </c>
+      <c r="L35">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>48</v>
       </c>
@@ -1802,8 +2090,17 @@
       <c r="I36">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36">
+        <v>0.63</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>49</v>
       </c>
@@ -1820,7 +2117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>50</v>
       </c>
@@ -1841,8 +2138,17 @@
       <c r="I38">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38">
+        <v>1.5</v>
+      </c>
+      <c r="K38">
+        <v>2.36</v>
+      </c>
+      <c r="L38">
+        <v>3.9279999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>51</v>
       </c>
@@ -1865,8 +2171,17 @@
       <c r="I39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39">
+        <v>1.125</v>
+      </c>
+      <c r="K39">
+        <v>1.3</v>
+      </c>
+      <c r="L39">
+        <v>2.7069999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>52</v>
       </c>
@@ -1883,7 +2198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>53</v>
       </c>
@@ -1904,8 +2219,17 @@
       <c r="I41">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41">
+        <v>1.5249999999999999</v>
+      </c>
+      <c r="K41">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="L41">
+        <v>5.0380000000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>55</v>
       </c>
@@ -1922,7 +2246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>56</v>
       </c>
@@ -1947,8 +2271,17 @@
       <c r="I43">
         <v>440</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <v>625</v>
+      </c>
+      <c r="K43">
+        <v>732</v>
+      </c>
+      <c r="L43">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>57</v>
       </c>
@@ -1967,8 +2300,17 @@
       <c r="I44">
         <v>36</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>44</v>
+      </c>
+      <c r="K44">
+        <v>48.2</v>
+      </c>
+      <c r="L44">
+        <v>54.12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>58</v>
       </c>
@@ -1989,8 +2331,17 @@
       <c r="I45">
         <v>95</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>100</v>
+      </c>
+      <c r="K45">
+        <v>112</v>
+      </c>
+      <c r="L45">
+        <v>125.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>59</v>
       </c>
@@ -2009,7 +2360,7 @@
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>60</v>
       </c>
@@ -2030,8 +2381,17 @@
       <c r="I47">
         <v>48</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <v>53</v>
+      </c>
+      <c r="K47">
+        <v>58.2</v>
+      </c>
+      <c r="L47">
+        <v>74.56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>62</v>
       </c>
@@ -2050,7 +2410,7 @@
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>63</v>
       </c>
@@ -2069,7 +2429,7 @@
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>64</v>
       </c>
@@ -2088,7 +2448,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>65</v>
       </c>
@@ -2107,7 +2467,7 @@
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>66</v>
       </c>
@@ -2126,7 +2486,7 @@
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>67</v>
       </c>
@@ -2145,7 +2505,7 @@
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>68</v>
       </c>
@@ -2164,7 +2524,7 @@
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>69</v>
       </c>
@@ -2183,7 +2543,7 @@
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>70</v>
       </c>
@@ -2204,8 +2564,17 @@
       <c r="I56">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J56">
+        <v>3.8</v>
+      </c>
+      <c r="K56">
+        <v>4.3</v>
+      </c>
+      <c r="L56">
+        <v>5.6879999999999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>71</v>
       </c>
@@ -2224,7 +2593,7 @@
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>72</v>
       </c>
@@ -2243,7 +2612,7 @@
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>73</v>
       </c>
@@ -2262,7 +2631,7 @@
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>74</v>
       </c>
@@ -2281,7 +2650,7 @@
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>75</v>
       </c>
@@ -2300,7 +2669,7 @@
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>76</v>
       </c>
@@ -2319,7 +2688,7 @@
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>77</v>
       </c>
@@ -2338,7 +2707,7 @@
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>78</v>
       </c>
@@ -2357,7 +2726,7 @@
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>79</v>
       </c>
@@ -2376,7 +2745,7 @@
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>80</v>
       </c>
@@ -2402,8 +2771,17 @@
       <c r="I66">
         <v>8.0500000000000002E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J66">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K66">
+        <v>0.2</v>
+      </c>
+      <c r="L66">
+        <v>0.31259999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>81</v>
       </c>
@@ -2424,8 +2802,17 @@
       <c r="I67">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J67">
+        <v>0.8</v>
+      </c>
+      <c r="K67">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="L67">
+        <v>1.2669999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>82</v>
       </c>
@@ -2453,8 +2840,17 @@
       <c r="I68">
         <v>18</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J68">
+        <v>22.5</v>
+      </c>
+      <c r="K68">
+        <v>28.8</v>
+      </c>
+      <c r="L68">
+        <v>41.94</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>83</v>
       </c>
@@ -2473,7 +2869,7 @@
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>90</v>
       </c>
@@ -2494,8 +2890,17 @@
       <c r="I70">
         <v>9.3000000000000007</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J70">
+        <v>10</v>
+      </c>
+      <c r="K70">
+        <v>11.8</v>
+      </c>
+      <c r="L70">
+        <v>17.059999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>92</v>
       </c>
@@ -2516,8 +2921,17 @@
       <c r="I71">
         <v>2.85</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J71">
+        <v>3.45</v>
+      </c>
+      <c r="K71">
+        <v>3.9</v>
+      </c>
+      <c r="L71">
+        <v>29.66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>999</v>
       </c>
@@ -2540,10 +2954,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMJ5"/>
+  <dimension ref="A1:AMJ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2573,7 +2987,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>147</v>
@@ -2581,10 +2995,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3"/>
       <c r="D3" s="2" t="s">
@@ -2596,7 +3010,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>156</v>
@@ -2606,19 +3020,52 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>158</v>
+      <c r="A5" t="s">
+        <v>162</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>157</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>